<commit_message>
Obtencion de codigo padre
</commit_message>
<xml_diff>
--- a/public/Expedientes/3__METRADOS_Y_PRESUPUESTO/NE_007---.xlsx
+++ b/public/Expedientes/3__METRADOS_Y_PRESUPUESTO/NE_007---.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvcs_pnvr_sasc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvcs_pnvr_sasc\Downloads\JUN EXP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -129,7 +129,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="_ [$S/.-280A]\ * #,##0.00_ ;_ [$S/.-280A]\ * \-#,##0.00_ ;_ [$S/.-280A]\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,11 +142,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -351,85 +346,88 @@
     <xf numFmtId="4" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="14" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="13" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -441,20 +439,21 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,16 +505,10 @@
       <sheetName val="HERRAMIENTAS"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="23">
-          <cell r="F23">
-            <v>42</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4">
         <row r="17">
           <cell r="B17">
@@ -1921,8 +1914,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
       <sheetData sheetId="7">
         <row r="43">
           <cell r="E43">
@@ -1937,12 +1930,12 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
       <sheetData sheetId="15">
         <row r="155">
           <cell r="E155">
@@ -1965,7 +1958,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="16"/>
       <sheetData sheetId="17">
         <row r="142">
           <cell r="D142">
@@ -1988,16 +1981,16 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2271,16 +2264,17 @@
   </sheetPr>
   <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="4.85546875" customWidth="1"/>
     <col min="4" max="4" width="82" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" customWidth="1"/>
-    <col min="6" max="7" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="9" max="11" width="11.42578125" customWidth="1"/>
   </cols>
@@ -2341,10 +2335,7 @@
         <f>'[1]RESU METRADO'!C18</f>
         <v>1</v>
       </c>
-      <c r="C3" s="7">
-        <f>'[1]RESU METRADO'!D18</f>
-        <v>0</v>
-      </c>
+      <c r="C3" s="7"/>
       <c r="D3" s="7" t="str">
         <f>'[1]RESU METRADO'!E18</f>
         <v xml:space="preserve">   TRABAJOS PRELIMINARES</v>
@@ -2405,10 +2396,7 @@
         <f>'[1]RESU METRADO'!C20</f>
         <v>2</v>
       </c>
-      <c r="C5" s="7">
-        <f>'[1]RESU METRADO'!D20</f>
-        <v>0</v>
-      </c>
+      <c r="C5" s="7"/>
       <c r="D5" s="7" t="str">
         <f>'[1]RESU METRADO'!E20</f>
         <v xml:space="preserve">   TRAZO NIVELES Y REPLANTEO PRELIMINAR</v>
@@ -2469,10 +2457,7 @@
         <f>'[1]RESU METRADO'!C22</f>
         <v>3</v>
       </c>
-      <c r="C7" s="7">
-        <f>'[1]RESU METRADO'!D22</f>
-        <v>0</v>
-      </c>
+      <c r="C7" s="7"/>
       <c r="D7" s="7" t="str">
         <f>'[1]RESU METRADO'!E22</f>
         <v xml:space="preserve">   SEGURIDAD Y SALUD</v>
@@ -4101,10 +4086,7 @@
         <f>'[1]RESU METRADO'!C73</f>
         <v>1</v>
       </c>
-      <c r="C58" s="7">
-        <f>'[1]RESU METRADO'!D73</f>
-        <v>0</v>
-      </c>
+      <c r="C58" s="7"/>
       <c r="D58" s="12" t="str">
         <f>'[1]RESU METRADO'!E73</f>
         <v>TARRAJEO VESTIDURAS Y DERRAMES</v>
@@ -5679,7 +5661,6 @@
       <c r="K112" s="36"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H112"/>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>

</xml_diff>